<commit_message>
Add pic of pinout
</commit_message>
<xml_diff>
--- a/Documentation/Atmega162 programmin pins.xlsx
+++ b/Documentation/Atmega162 programmin pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdvardOlaf\Documents\studier\5semester\byggern\byggern-TTK4155\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7E7C2C1D-97CE-4214-AEEE-103A74AC4761}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2A7E658A-46EA-4CB1-83C4-37CE20CCA0BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="8448" xr2:uid="{AE3FA2CD-5865-4833-8004-B36A80CAC1B7}"/>
   </bookViews>
@@ -116,6 +116,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>743835</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>132465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238578</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>93798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Bilde 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8174E4FC-ED00-4CE4-BE54-057C5B3A5F2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1409700" y="1402080"/>
+          <a:ext cx="4533333" cy="3457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,7 +467,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,5 +558,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>